<commit_message>
save new xlsx with later tests as well as gitignore
</commit_message>
<xml_diff>
--- a/Data/CompressionTest_1999Camry(Mk3).xlsx
+++ b/Data/CompressionTest_1999Camry(Mk3).xlsx
@@ -3,9 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Test1" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Test2" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="Notes" sheetId="3" r:id="rId5"/>
+    <sheet state="visible" name="1717 (Test1)" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="1717 (Test2)" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="21117 (Test3)" sheetId="3" r:id="rId5"/>
+    <sheet state="visible" name="21217 (Corolla)" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="Notes" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +15,76 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
+  <si>
+    <t>Dry Test</t>
+  </si>
+  <si>
+    <t>Wet Test</t>
+  </si>
+  <si>
+    <t>Stroke</t>
+  </si>
+  <si>
+    <t>Cylinder #1</t>
+  </si>
+  <si>
+    <t>Cylinder #2</t>
+  </si>
+  <si>
+    <t>Cylinder #3</t>
+  </si>
+  <si>
+    <t>Cylinder #4</t>
+  </si>
+  <si>
+    <t>Cyliner #1</t>
+  </si>
+  <si>
+    <t>Cyliner #2</t>
+  </si>
+  <si>
+    <t>Cylinder #2 1st</t>
+  </si>
+  <si>
+    <t>"Visual" Maximum</t>
+  </si>
+  <si>
+    <t>Might have started TDC and first stroke is 35</t>
+  </si>
+  <si>
+    <t>first stroke 50</t>
+  </si>
+  <si>
+    <t>Extras</t>
+  </si>
+  <si>
+    <t>Cylinder #2 (Dry Test 1)</t>
+  </si>
+  <si>
+    <t>Cylinder #4 (Wet Test 1)</t>
+  </si>
+  <si>
+    <t>Cylinder #4 (Wet Test 2)</t>
+  </si>
+  <si>
+    <t>"Visual" Max:</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Camera angle skews accuracy</t>
+  </si>
+  <si>
+    <t>Guage fell out of view during test</t>
+  </si>
+  <si>
+    <t>Not enough oil in cylinder</t>
+  </si>
+  <si>
+    <t>Camera was dark and out of focus for all wet tests</t>
+  </si>
   <si>
     <t>Compression tests were done in cylinder order 4-3-2-1 for all tests</t>
   </si>
@@ -42,43 +113,7 @@
     <t>In second compression test series, cylinder #3 has very low pressure step at beginning that doesnt sound like a stroke but may be a very weak one</t>
   </si>
   <si>
-    <t>Dry Test</t>
-  </si>
-  <si>
-    <t>Wet Test</t>
-  </si>
-  <si>
-    <t>Stroke</t>
-  </si>
-  <si>
-    <t>Cylinder #1</t>
-  </si>
-  <si>
-    <t>Cylinder #2</t>
-  </si>
-  <si>
-    <t>Cylinder #3</t>
-  </si>
-  <si>
-    <t>Cylinder #4</t>
-  </si>
-  <si>
-    <t>Cyliner #1</t>
-  </si>
-  <si>
-    <t>Cyliner #2</t>
-  </si>
-  <si>
-    <t>Cylinder #2 1st</t>
-  </si>
-  <si>
-    <t>"Visual" Maximum</t>
-  </si>
-  <si>
-    <t>Might have started TDC and first stroke is 35</t>
-  </si>
-  <si>
-    <t>first stroke 50</t>
+    <t>Third compression test is after seafoam engine cleaning treatment</t>
   </si>
 </sst>
 </file>
@@ -127,15 +162,23 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/worksheetdrawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/worksheetdrawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -149,45 +192,45 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -452,7 +495,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1">
         <v>205.0</v>
@@ -501,42 +544,42 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -956,7 +999,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B24" s="1">
         <v>215.0</v>
@@ -985,10 +1028,10 @@
     </row>
     <row r="26">
       <c r="D26" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1004,48 +1047,1288 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>62.0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>56.0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>58.0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>90.0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>91.0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>79.0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>84.0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>83.0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>74.0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>79.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>134.0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>116.0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>117.0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>125.0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>145.0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>130.0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>130.0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>151.0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>126.0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>122.0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>138.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>160.0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>144.0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>146.0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>154.0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>178.0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>165.0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>165.0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>185.0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>155.0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>151.0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>176.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>178.0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>165.0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>169.0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>172.0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>190.0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>188.0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>206.0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>174.0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>172.0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>201.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>188.0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>179.0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>183.0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>183.0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>216.0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>206.0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>204.0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>220.0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>184.0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>186.0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>211.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>195.0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>186.0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>190.0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>190.0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>229.0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>218.0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>213.0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>230.0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>192.0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>195.0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>235.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>202.0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>194.0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>198.0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>198.0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>236.0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>226.0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>228.0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>236.0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>196.0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>244.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>207.0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>199.0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>204.0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>242.0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>231.0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>231.0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>241.0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>201.0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>205.0</v>
+      </c>
+      <c r="N10" s="1">
+        <v>250.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>209.0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>203.0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>208.0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>203.0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>246.0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>235.0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>234.0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>244.0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>210.0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>255.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="B12" s="1">
+        <v>213.0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>205.0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>210.0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>205.0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>250.0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>239.0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>236.0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>246.0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>211.0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>259.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="B13" s="1">
+        <v>215.0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>205.0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>211.0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>207.0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>250.0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>240.0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>237.0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>248.0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>213.0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>260.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>216.0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>207.0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>212.0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>209.0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>251.0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>241.0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>238.0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>250.0</v>
+      </c>
+      <c r="N14" s="1">
+        <v>261.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="B15" s="1">
+        <v>216.0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>208.0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>214.0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>210.0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>252.0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>242.0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>240.0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>252.0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>263.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="B16" s="1">
+        <v>217.0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>209.0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>215.0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>253.0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>243.0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>241.0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>253.0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>265.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>210.0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>254.0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>244.0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>243.0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>253.0</v>
+      </c>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>210.0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>254.0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>245.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1">
+        <v>250.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="L26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>95.0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>90.0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>105.0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>105.0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>146.0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>139.0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>145.0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>155.0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>156.0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>155.0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>155.0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>160.0</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>166.0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>160.0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>164.0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>170.0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>179.0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>179.0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>180.0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>190.0</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>185.0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>177.0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>182.0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>190.0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>199.0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>200.0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>215.0</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>197.0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>190.0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>193.0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>204.0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>212.0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>215.0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>215.0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>231.0</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>206.0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>109.0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>201.0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>212.0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>221.0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>224.0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>228.0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>241.0</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>212.0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>204.0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>207.0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>219.0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>227.0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>231.0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>234.0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>248.0</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>216.0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>207.0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>211.0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>224.0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>232.0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>234.0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>239.0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>255.0</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>220.0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>210.0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>214.0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>226.0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>235.0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>237.0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>244.0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>259.0</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="B12" s="1">
+        <v>222.0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>213.0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>216.0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>229.0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>237.0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>238.0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>245.0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>262.0</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="B13" s="1">
+        <v>223.0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>214.0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>218.0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>230.0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>238.0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>239.0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>247.0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>263.0</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>224.0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>215.0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>219.0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>231.0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>239.0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>239.0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>249.0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>264.0</v>
+      </c>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="B15" s="1">
+        <v>224.0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>215.0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>219.0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>231.0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>239.0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>239.0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>249.0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>264.0</v>
+      </c>
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="B16" s="1">
+        <v>225.0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>216.0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>220.0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>231.0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>239.0</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1">
+        <v>248.0</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>216.0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>220.0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>231.0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>239.0</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1">
+        <v>247.0</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>216.0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>220.0</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>17.0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>216.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>216.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="G26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>